<commit_message>
Feat : Enemy Spawner 구현
WaveSO -> 각 스테이지 별로 출현 가능한 몬스터의 종류 및 Spawn에 필요한 변수들을 저장해두는 SO
</commit_message>
<xml_diff>
--- a/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6110F4C-529A-4D15-A75F-0576E1324958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF8564A-AE13-4920-B110-4CBA5F498378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="2610" yWindow="7455" windowWidth="29475" windowHeight="16005" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -652,7 +652,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -663,7 +663,7 @@
     <col min="4" max="4" width="48" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.25" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" style="2" bestFit="1" customWidth="1"/>
@@ -1059,7 +1059,7 @@
         <v>22</v>
       </c>
       <c r="G9" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H9" s="2">
         <v>2.2999999999999998</v>
@@ -1106,7 +1106,7 @@
         <v>21</v>
       </c>
       <c r="G10" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H10" s="2">
         <v>3</v>
@@ -1153,7 +1153,7 @@
         <v>21</v>
       </c>
       <c r="G11" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H11" s="2">
         <v>2.5</v>
@@ -1247,7 +1247,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H13" s="2">
         <v>3</v>
@@ -1294,7 +1294,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H14" s="2">
         <v>2</v>
@@ -1341,7 +1341,7 @@
         <v>22</v>
       </c>
       <c r="G15" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H15" s="2">
         <v>10</v>
@@ -1388,7 +1388,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="2">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H16" s="2">
         <v>20</v>

</xml_diff>

<commit_message>
Feat : AreaAttack 수정
투사체처럼 id값을 가지게 변경.
</commit_message>
<xml_diff>
--- a/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412E42BA-878B-4DE8-BB12-AE4612CFBAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82A7D8A-1252-4DD2-8C26-DBCB878B26FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
@@ -672,7 +672,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1506,10 +1506,10 @@
         <v>53</v>
       </c>
       <c r="G18" s="2">
-        <v>600</v>
+        <v>100000</v>
       </c>
       <c r="H18" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -1521,7 +1521,7 @@
         <v>5</v>
       </c>
       <c r="L18" s="2">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="M18" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
Feat : Rune UI 구현 및 코드 개선
</commit_message>
<xml_diff>
--- a/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50E9FF3-AE25-4AE5-9A14-A81F98303FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A73623-E35B-4751-8DC7-6BABC93A710D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
@@ -672,7 +672,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1474,7 +1474,7 @@
         <v>0.3</v>
       </c>
       <c r="M17" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N17" s="2">
         <v>2</v>
@@ -1524,13 +1524,13 @@
         <v>0.6</v>
       </c>
       <c r="M18" s="2">
+        <v>10</v>
+      </c>
+      <c r="N18" s="2">
+        <v>3</v>
+      </c>
+      <c r="O18" s="2">
         <v>5</v>
-      </c>
-      <c r="N18" s="2">
-        <v>3</v>
-      </c>
-      <c r="O18" s="2">
-        <v>4</v>
       </c>
       <c r="Q18" s="2">
         <v>0.5</v>
@@ -1580,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="O19" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat : 강화 UI구현
</commit_message>
<xml_diff>
--- a/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A73623-E35B-4751-8DC7-6BABC93A710D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2708B9B-7AF6-4C01-81FE-C45089BC5766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
   <si>
     <t>Normal</t>
   </si>
@@ -243,6 +243,14 @@
   </si>
   <si>
     <t>Enemy/Prefabs/Boss/Enemy_EvilMage_Boss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -672,7 +680,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -741,6 +749,9 @@
       <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -788,6 +799,9 @@
       </c>
       <c r="O2" s="2">
         <v>3</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Style : Enemt 의 meleeAttack -> physicalAtk로 변경
</commit_message>
<xml_diff>
--- a/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2708B9B-7AF6-4C01-81FE-C45089BC5766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F7DD8-0802-4E51-94EB-C79D0E413245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t>Normal</t>
   </si>
@@ -53,10 +53,6 @@
     <t>TurtleShell</t>
   </si>
   <si>
-    <t>Player Radius</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Small</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -85,10 +81,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>meleeAtk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>magicAtk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -246,12 +238,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,2,3,4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>physicalAtk</t>
   </si>
 </sst>
 </file>
@@ -299,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +320,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -342,6 +335,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,7 +676,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -693,7 +689,8 @@
     <col min="6" max="6" width="8.625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.75" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="2" bestFit="1" customWidth="1"/>
@@ -705,52 +702,49 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>55</v>
+      <c r="O1" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="Q1" s="4"/>
     </row>
@@ -759,19 +753,19 @@
         <v>30000000</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2">
         <v>20</v>
@@ -799,9 +793,6 @@
       </c>
       <c r="O2" s="2">
         <v>3</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -815,10 +806,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="2">
         <v>50</v>
@@ -859,10 +850,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2">
         <v>700</v>
@@ -897,19 +888,19 @@
         <v>30100000</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -950,10 +941,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" s="2">
         <v>50</v>
@@ -994,10 +985,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G7" s="2">
         <v>700</v>
@@ -1032,19 +1023,19 @@
         <v>30200000</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G8" s="2">
         <v>20</v>
@@ -1079,19 +1070,19 @@
         <v>30300000</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G9" s="2">
         <v>30</v>
@@ -1126,19 +1117,19 @@
         <v>30310001</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G10" s="2">
         <v>100</v>
@@ -1173,19 +1164,19 @@
         <v>30400001</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G11" s="2">
         <v>50</v>
@@ -1220,19 +1211,19 @@
         <v>30420001</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G12" s="2">
         <v>100000</v>
@@ -1267,19 +1258,19 @@
         <v>30600000</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G13" s="2">
         <v>20</v>
@@ -1314,19 +1305,19 @@
         <v>30700000</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G14" s="2">
         <v>50</v>
@@ -1361,19 +1352,19 @@
         <v>30700001</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G15" s="2">
         <v>50</v>
@@ -1408,19 +1399,19 @@
         <v>30800000</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G16" s="2">
         <v>30</v>
@@ -1450,24 +1441,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>30900000</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G17" s="2">
         <v>30</v>
@@ -1496,28 +1487,25 @@
       <c r="O17" s="2">
         <v>3</v>
       </c>
-      <c r="Q17" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>30920003</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G18" s="2">
         <v>300</v>
@@ -1546,28 +1534,25 @@
       <c r="O18" s="2">
         <v>5</v>
       </c>
-      <c r="Q18" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>31000000</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G19" s="2">
         <v>100</v>

</xml_diff>

<commit_message>
Feat : Enemy Spawn 위치 유효성 검사 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F7DD8-0802-4E51-94EB-C79D0E413245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F8317E-0148-4692-B517-33E0FE361E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
   <si>
     <t>Normal</t>
   </si>
@@ -219,10 +219,6 @@
   </si>
   <si>
     <t>Enemy/Prefabs/Elite/Enemy_Skeleton_Elite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Large</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -676,7 +672,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -726,7 +722,7 @@
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -1176,7 +1172,7 @@
         <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="G11" s="2">
         <v>50</v>
@@ -1217,13 +1213,13 @@
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="G12" s="2">
         <v>100000</v>
@@ -1496,16 +1492,16 @@
         <v>45</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G18" s="2">
         <v>300</v>

</xml_diff>

<commit_message>
Feat : FieldItem 오브젝트풀 적용
</commit_message>
<xml_diff>
--- a/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DDDC55-FD36-41A4-84B1-1D2407440B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78491ACD-CD63-4451-A17F-ED0BBE21B292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>Normal</t>
   </si>
@@ -235,6 +235,10 @@
   </si>
   <si>
     <t>physicalAtk</t>
+  </si>
+  <si>
+    <t>gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -672,7 +676,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -742,6 +746,9 @@
       <c r="O1" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="P1" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -790,6 +797,9 @@
       <c r="O2" s="2">
         <v>3</v>
       </c>
+      <c r="P2" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -834,6 +844,9 @@
       <c r="O3" s="2">
         <v>3</v>
       </c>
+      <c r="P3" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -878,6 +891,9 @@
       <c r="O4" s="2">
         <v>3</v>
       </c>
+      <c r="P4" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -925,6 +941,9 @@
       <c r="O5" s="2">
         <v>3</v>
       </c>
+      <c r="P5" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -969,6 +988,9 @@
       <c r="O6" s="2">
         <v>3</v>
       </c>
+      <c r="P6" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -1013,6 +1035,9 @@
       <c r="O7" s="2">
         <v>3</v>
       </c>
+      <c r="P7" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -1060,6 +1085,9 @@
       <c r="O8" s="2">
         <v>3</v>
       </c>
+      <c r="P8" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -1107,6 +1135,9 @@
       <c r="O9" s="2">
         <v>3</v>
       </c>
+      <c r="P9" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -1154,6 +1185,9 @@
       <c r="O10" s="2">
         <v>4</v>
       </c>
+      <c r="P10" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -1201,6 +1235,9 @@
       <c r="O11" s="2">
         <v>3</v>
       </c>
+      <c r="P11" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -1248,6 +1285,9 @@
       <c r="O12" s="2">
         <v>4</v>
       </c>
+      <c r="P12" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
@@ -1295,6 +1335,9 @@
       <c r="O13" s="2">
         <v>3</v>
       </c>
+      <c r="P13" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
@@ -1342,6 +1385,9 @@
       <c r="O14" s="2">
         <v>3</v>
       </c>
+      <c r="P14" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
@@ -1389,6 +1435,9 @@
       <c r="O15" s="2">
         <v>3</v>
       </c>
+      <c r="P15" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
@@ -1436,8 +1485,11 @@
       <c r="O16" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>30900000</v>
       </c>
@@ -1483,8 +1535,11 @@
       <c r="O17" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>30920003</v>
       </c>
@@ -1530,8 +1585,11 @@
       <c r="O18" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>31000000</v>
       </c>
@@ -1576,6 +1634,9 @@
       </c>
       <c r="O19" s="2">
         <v>6</v>
+      </c>
+      <c r="P19" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat : 메뉴 Esc 수정
</commit_message>
<xml_diff>
--- a/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/Enemy/EnemyDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A62BA62-9C7A-4A39-9A62-16189E6E7E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB25AC02-1833-4DFA-82F9-CC79500DB43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="2055" yWindow="2085" windowWidth="33855" windowHeight="16470" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -676,7 +676,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1259,7 +1259,7 @@
         <v>50</v>
       </c>
       <c r="G12" s="2">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="H12" s="2">
         <v>6</v>
@@ -1559,7 +1559,7 @@
         <v>50</v>
       </c>
       <c r="G18" s="2">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="H18" s="2">
         <v>15</v>

</xml_diff>